<commit_message>
3D model behaves again
</commit_message>
<xml_diff>
--- a/support/Bright Eyes.xlsx
+++ b/support/Bright Eyes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bromptonbicycleuk-my.sharepoint.com/personal/joel_santos_brompton_co_uk/Documents/Desktop/Calavera/Support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bromptonbicycleuk-my.sharepoint.com/personal/joel_santos_brompton_co_uk/Documents/Desktop/Calavera/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{17172B75-C90D-493A-A0BE-3F9CEEBB8B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A172951F-67B9-44D2-99E3-4DF84619EDDA}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{17172B75-C90D-493A-A0BE-3F9CEEBB8B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A785812B-B5DB-4249-9A95-AE17E8765DAF}"/>
   <bookViews>
-    <workbookView xWindow="-3765" yWindow="4260" windowWidth="21600" windowHeight="11835" xr2:uid="{EA40F893-9D77-4B88-B27A-E56D36ACA1DC}"/>
+    <workbookView minimized="1" xWindow="-24465" yWindow="3390" windowWidth="21600" windowHeight="11835" xr2:uid="{EA40F893-9D77-4B88-B27A-E56D36ACA1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
         <v>1470</v>
       </c>
       <c r="D3">
-        <v>1470</v>
+        <v>1500</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -627,7 +627,7 @@
       </c>
       <c r="D10" s="4">
         <f>1/(4*D$2*D$5)*(D$4/D$3)</f>
-        <v>0.38651824366110082</v>
+        <v>0.37878787878787884</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
       </c>
       <c r="D12" s="1">
         <f>(1/D10)*(1-D6)</f>
-        <v>0.51578286629303438</v>
+        <v>0.52630904723779015</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="D13" s="1">
         <f>(1/D10)*D6</f>
-        <v>2.0714171337069653</v>
+        <v>2.1136909527622096</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>